<commit_message>
bug fix of doc
</commit_message>
<xml_diff>
--- a/docmed.xlsx
+++ b/docmed.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -567,6 +567,20 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>bjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>